<commit_message>
Análises por regiao, regressao por regiao
</commit_message>
<xml_diff>
--- a/dados/dados brutos/IDEB Paraíba.xlsx
+++ b/dados/dados brutos/IDEB Paraíba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Serie/ano: Todas</t>
   </si>
   <si>
-    <t xml:space="preserve">Município</t>
+    <t xml:space="preserve">Municipio</t>
   </si>
   <si>
     <t xml:space="preserve">2007 - META</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">2021 – META</t>
   </si>
   <si>
-    <t xml:space="preserve">Caldas Brandão</t>
+    <t xml:space="preserve">Caldas Brandao</t>
   </si>
   <si>
     <t xml:space="preserve">Boa Vista</t>
@@ -73,10 +73,10 @@
     <t xml:space="preserve">Monteiro</t>
   </si>
   <si>
-    <t xml:space="preserve">Água Branca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esperança</t>
+    <t xml:space="preserve">agua Branca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esperanca</t>
   </si>
   <si>
     <t xml:space="preserve">Carrapateira</t>
@@ -85,10 +85,10 @@
     <t xml:space="preserve">Montadas</t>
   </si>
   <si>
-    <t xml:space="preserve">Olho d'Água</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Mamede</t>
+    <t xml:space="preserve">Olho dagua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Mamede</t>
   </si>
   <si>
     <t xml:space="preserve">Bom Sucesso</t>
@@ -103,22 +103,22 @@
     <t xml:space="preserve">Serra Branca</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonito de Santa Fé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dona Inês</t>
+    <t xml:space="preserve">Bonito de Santa Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dona Ines</t>
   </si>
   <si>
     <t xml:space="preserve">Lagoa de Dentro</t>
   </si>
   <si>
-    <t xml:space="preserve">Marizópolis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santa Inês</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caturité</t>
+    <t xml:space="preserve">Marizopolis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Ines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caturite</t>
   </si>
   <si>
     <t xml:space="preserve">Ibiara</t>
@@ -127,31 +127,31 @@
     <t xml:space="preserve">Pombal</t>
   </si>
   <si>
-    <t xml:space="preserve">Tenório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zabelê</t>
+    <t xml:space="preserve">Tenorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zabele</t>
   </si>
   <si>
     <t xml:space="preserve">Aparecida</t>
   </si>
   <si>
-    <t xml:space="preserve">Camalaú</t>
+    <t xml:space="preserve">Camalau</t>
   </si>
   <si>
     <t xml:space="preserve">Campina Grande</t>
   </si>
   <si>
-    <t xml:space="preserve">Catolé do Rocha</t>
+    <t xml:space="preserve">Catole do Rocha</t>
   </si>
   <si>
     <t xml:space="preserve">Mogeiro</t>
   </si>
   <si>
-    <t xml:space="preserve">São Bentinho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baía da Traição</t>
+    <t xml:space="preserve">Sao Bentinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baia da Traicao</t>
   </si>
   <si>
     <t xml:space="preserve">Barra de Santana</t>
@@ -175,28 +175,28 @@
     <t xml:space="preserve">Paulista</t>
   </si>
   <si>
-    <t xml:space="preserve">São João do Cariri</t>
+    <t xml:space="preserve">Sao Joao do Cariri</t>
   </si>
   <si>
     <t xml:space="preserve">Serra Grande</t>
   </si>
   <si>
-    <t xml:space="preserve">Caaporã</t>
+    <t xml:space="preserve">Caapora</t>
   </si>
   <si>
     <t xml:space="preserve">Itabaiana</t>
   </si>
   <si>
-    <t xml:space="preserve">João Pessoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puxinanã</t>
+    <t xml:space="preserve">Joao Pessoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puxinana</t>
   </si>
   <si>
     <t xml:space="preserve">Queimadas</t>
   </si>
   <si>
-    <t xml:space="preserve">São Sebastião de Lagoa de Roça</t>
+    <t xml:space="preserve">Sao Sebastiao de Lagoa de Roca</t>
   </si>
   <si>
     <t xml:space="preserve">Serra da Raiz</t>
@@ -229,13 +229,13 @@
     <t xml:space="preserve">Prata</t>
   </si>
   <si>
-    <t xml:space="preserve">São Francisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Miguel de Taipu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumé</t>
+    <t xml:space="preserve">Sao Francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Miguel de Taipu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sume</t>
   </si>
   <si>
     <t xml:space="preserve">Tavares</t>
@@ -244,10 +244,10 @@
     <t xml:space="preserve">Areia</t>
   </si>
   <si>
-    <t xml:space="preserve">Conceição</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cruz do Espírito Santo</t>
+    <t xml:space="preserve">Conceicao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruz do Espirito Santo</t>
   </si>
   <si>
     <t xml:space="preserve">Curral de Cima</t>
@@ -286,7 +286,7 @@
     <t xml:space="preserve">Araruna</t>
   </si>
   <si>
-    <t xml:space="preserve">Boqueirão</t>
+    <t xml:space="preserve">Boqueirao</t>
   </si>
   <si>
     <t xml:space="preserve">Brejo do Cruz</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Itatuba</t>
   </si>
   <si>
-    <t xml:space="preserve">Jericó</t>
+    <t xml:space="preserve">Jerico</t>
   </si>
   <si>
     <t xml:space="preserve">Lagoa Seca</t>
@@ -316,40 +316,40 @@
     <t xml:space="preserve">Pedra Branca</t>
   </si>
   <si>
-    <t xml:space="preserve">Picuí</t>
+    <t xml:space="preserve">Picui</t>
   </si>
   <si>
     <t xml:space="preserve">Princesa Isabel</t>
   </si>
   <si>
-    <t xml:space="preserve">São José do Brejo do Cruz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Sebastião do Umbuzeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uiraúna</t>
+    <t xml:space="preserve">Sao Jose do Brejo do Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Sebastiao do Umbuzeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uirauna</t>
   </si>
   <si>
     <t xml:space="preserve">Aroeiras</t>
   </si>
   <si>
-    <t xml:space="preserve">Baraúna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barra de São Miguel</t>
+    <t xml:space="preserve">Barauna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barra de Sao Miguel</t>
   </si>
   <si>
     <t xml:space="preserve">Bayeux</t>
   </si>
   <si>
-    <t xml:space="preserve">Belém</t>
+    <t xml:space="preserve">Belem</t>
   </si>
   <si>
     <t xml:space="preserve">Brejo dos Santos</t>
   </si>
   <si>
-    <t xml:space="preserve">Caiçara</t>
+    <t xml:space="preserve">Caicara</t>
   </si>
   <si>
     <t xml:space="preserve">Massaranduba</t>
@@ -364,13 +364,13 @@
     <t xml:space="preserve">Pirpirituba</t>
   </si>
   <si>
-    <t xml:space="preserve">Riachão</t>
+    <t xml:space="preserve">Riachao</t>
   </si>
   <si>
     <t xml:space="preserve">Santa Cruz</t>
   </si>
   <si>
-    <t xml:space="preserve">São José do Sabugi</t>
+    <t xml:space="preserve">Sao Jose do Sabugi</t>
   </si>
   <si>
     <t xml:space="preserve">Bananeiras</t>
@@ -385,16 +385,16 @@
     <t xml:space="preserve">Coremas</t>
   </si>
   <si>
-    <t xml:space="preserve">Damião</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Junco do Seridó</t>
+    <t xml:space="preserve">Damiao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junco do Serido</t>
   </si>
   <si>
     <t xml:space="preserve">Juripiranga</t>
   </si>
   <si>
-    <t xml:space="preserve">Pilõezinhos</t>
+    <t xml:space="preserve">Piloezinhos</t>
   </si>
   <si>
     <t xml:space="preserve">Pocinhos</t>
@@ -409,13 +409,13 @@
     <t xml:space="preserve">Santa Luzia</t>
   </si>
   <si>
-    <t xml:space="preserve">São José do Bonfim</t>
+    <t xml:space="preserve">Sao Jose do Bonfim</t>
   </si>
   <si>
     <t xml:space="preserve">Sobrado</t>
   </si>
   <si>
-    <t xml:space="preserve">Solânea</t>
+    <t xml:space="preserve">Solanea</t>
   </si>
   <si>
     <t xml:space="preserve">Cuitegi</t>
@@ -424,10 +424,10 @@
     <t xml:space="preserve">Duas Estradas</t>
   </si>
   <si>
-    <t xml:space="preserve">Juarez Távora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maturéia</t>
+    <t xml:space="preserve">Juarez Tavora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matureia</t>
   </si>
   <si>
     <t xml:space="preserve">Nazarezinho</t>
@@ -436,7 +436,7 @@
     <t xml:space="preserve">Pilar</t>
   </si>
   <si>
-    <t xml:space="preserve">Remígio</t>
+    <t xml:space="preserve">Remigio</t>
   </si>
   <si>
     <t xml:space="preserve">Santa Rita</t>
@@ -451,22 +451,22 @@
     <t xml:space="preserve">Barra de Santa Rosa</t>
   </si>
   <si>
-    <t xml:space="preserve">Cachoeira dos Índios</t>
+    <t xml:space="preserve">Cachoeira dos indios</t>
   </si>
   <si>
     <t xml:space="preserve">Catingueira</t>
   </si>
   <si>
-    <t xml:space="preserve">Cuité de Mamanguape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacaraú</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mãe d'Água</t>
+    <t xml:space="preserve">Cuite de Mamanguape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacarau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mae dagua</t>
   </si>
   <si>
     <t xml:space="preserve">Mulungu</t>
@@ -478,10 +478,10 @@
     <t xml:space="preserve">Nova Palmeira</t>
   </si>
   <si>
-    <t xml:space="preserve">Riachão do Bacamarte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José de Piranhas</t>
+    <t xml:space="preserve">Riachao do Bacamarte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose de Piranhas</t>
   </si>
   <si>
     <t xml:space="preserve">Serra Redonda</t>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">Soledade</t>
   </si>
   <si>
-    <t xml:space="preserve">Sossêgo</t>
+    <t xml:space="preserve">Sossego</t>
   </si>
   <si>
     <t xml:space="preserve">Teixeira</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">Arara</t>
   </si>
   <si>
-    <t xml:space="preserve">Assunção</t>
+    <t xml:space="preserve">Assuncao</t>
   </si>
   <si>
     <t xml:space="preserve">Cajazeiras</t>
@@ -511,13 +511,13 @@
     <t xml:space="preserve">Capim</t>
   </si>
   <si>
-    <t xml:space="preserve">Cuité</t>
+    <t xml:space="preserve">Cuite</t>
   </si>
   <si>
     <t xml:space="preserve">Mamanguape</t>
   </si>
   <si>
-    <t xml:space="preserve">Manaíra</t>
+    <t xml:space="preserve">Manaira</t>
   </si>
   <si>
     <t xml:space="preserve">Mataraca</t>
@@ -529,31 +529,31 @@
     <t xml:space="preserve">Pedras de Fogo</t>
   </si>
   <si>
-    <t xml:space="preserve">Piancó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poço de José de Moura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José dos Ramos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sapé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Araçagi</t>
+    <t xml:space="preserve">Pianco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poco de Jose de Moura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose dos Ramos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aracagi</t>
   </si>
   <si>
     <t xml:space="preserve">Cacimbas</t>
   </si>
   <si>
-    <t xml:space="preserve">Gurinhém</t>
+    <t xml:space="preserve">Gurinhem</t>
   </si>
   <si>
     <t xml:space="preserve">Imaculada</t>
   </si>
   <si>
-    <t xml:space="preserve">Riachão do Poço</t>
+    <t xml:space="preserve">Riachao do Poco</t>
   </si>
   <si>
     <t xml:space="preserve">Riacho dos Cavalos</t>
@@ -562,13 +562,13 @@
     <t xml:space="preserve">Serraria</t>
   </si>
   <si>
-    <t xml:space="preserve">Belém do Brejo do Cruz</t>
+    <t xml:space="preserve">Belem do Brejo do Cruz</t>
   </si>
   <si>
     <t xml:space="preserve">Itapororoca</t>
   </si>
   <si>
-    <t xml:space="preserve">São José da Lagoa Tapada</t>
+    <t xml:space="preserve">Sao Jose da Lagoa Tapada</t>
   </si>
   <si>
     <t xml:space="preserve">Tacima</t>
@@ -580,7 +580,7 @@
     <t xml:space="preserve">Condado</t>
   </si>
   <si>
-    <t xml:space="preserve">Marcação</t>
+    <t xml:space="preserve">Marcacao</t>
   </si>
   <si>
     <t xml:space="preserve">Pedra Lavrada</t>
@@ -589,22 +589,22 @@
     <t xml:space="preserve">Pitimbu</t>
   </si>
   <si>
-    <t xml:space="preserve">São Bento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pilões</t>
+    <t xml:space="preserve">Sao Bento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piloes</t>
   </si>
   <si>
     <t xml:space="preserve">Aguiar</t>
   </si>
   <si>
-    <t xml:space="preserve">Algodão de Jandaíra</t>
+    <t xml:space="preserve">Algodao de Jandaira</t>
   </si>
   <si>
     <t xml:space="preserve">Amparo</t>
   </si>
   <si>
-    <t xml:space="preserve">Areia de Baraúnas</t>
+    <t xml:space="preserve">Areia de Baraunas</t>
   </si>
   <si>
     <t xml:space="preserve">**</t>
@@ -616,7 +616,7 @@
     <t xml:space="preserve">Cajazeirinhas</t>
   </si>
   <si>
-    <t xml:space="preserve">Caraúbas</t>
+    <t xml:space="preserve">Caraubas</t>
   </si>
   <si>
     <t xml:space="preserve">Coxixola</t>
@@ -631,7 +631,7 @@
     <t xml:space="preserve">Gado Bravo</t>
   </si>
   <si>
-    <t xml:space="preserve">Gurjão</t>
+    <t xml:space="preserve">Gurjao</t>
   </si>
   <si>
     <t xml:space="preserve">Igaracy</t>
@@ -667,73 +667,73 @@
     <t xml:space="preserve">Passagem</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro Régis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poço Dantas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quixabá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riacho de Santo Antônio</t>
+    <t xml:space="preserve">Pedro Regis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poco Dantas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quixaba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riacho de Santo Antonio</t>
   </si>
   <si>
     <t xml:space="preserve">Salgadinho</t>
   </si>
   <si>
-    <t xml:space="preserve">Salgado de São Félix</t>
+    <t xml:space="preserve">Salgado de Sao Felix</t>
   </si>
   <si>
     <t xml:space="preserve">*</t>
   </si>
   <si>
-    <t xml:space="preserve">Santa Cecília</t>
+    <t xml:space="preserve">Santa Cecilia</t>
   </si>
   <si>
     <t xml:space="preserve">Santana de Mangueira</t>
   </si>
   <si>
-    <t xml:space="preserve">Santo André</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Domingos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Domingos do Cariri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São João do Rio do Peixe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São João do Tigre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José de Caiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José de Espinharas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José de Princesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São José dos Cordeiros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Vicente do Seridó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sertãozinho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taperoá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Várzea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vieirópolis</t>
+    <t xml:space="preserve">Santo Andre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Domingos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Domingos do Cariri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Joao do Rio do Peixe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Joao do Tigre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose de Caiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose de Espinharas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose de Princesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Jose dos Cordeiros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Vicente do Serido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sertaozinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taperoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varzea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vieiropolis</t>
   </si>
   <si>
     <t xml:space="preserve">Vista Serrana</t>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="11" sqref="A6 A31 A46 A62 A97 A148 A158 A161 A165 A174 A203 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1077,8 +1077,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="11" sqref="A6 A31 A46 A62 A97 A148 A158 A161 A165 A174 A203 A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11949,8 +11949,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A108" activeCellId="11" sqref="A6 A31 A46 A62 A97 A148 A158 A161 A165 A174 A203 A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22165,7 +22165,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="11" sqref="A6 A31 A46 A62 A97 A148 A158 A161 A165 A174 A203 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>